<commit_message>
las recompilation. Still the problem with the rasterbar is not controlled...
</commit_message>
<xml_diff>
--- a/docs/HexaDec.xlsx
+++ b/docs/HexaDec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5C51E2-9BE6-4A2D-9878-AEFBD85DA221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326A4F39-2EEE-4977-9B7B-7A2B123A2E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{C70C2E63-9336-4B10-BFD2-FFF09962B0E6}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
-  <si>
-    <t>Conversor</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Decimal</t>
   </si>
@@ -47,9 +44,6 @@
     <t>Hexadecimal</t>
   </si>
   <si>
-    <t>Binario</t>
-  </si>
-  <si>
     <t>Operation</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>Result</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
@@ -78,6 +69,21 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>Conversion</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>080d</t>
+  </si>
+  <si>
+    <t>081a</t>
+  </si>
+  <si>
+    <t>0d</t>
   </si>
 </sst>
 </file>
@@ -156,13 +162,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,124 +507,124 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B3" s="5" t="str">
         <f>DEC2HEX(A3)</f>
-        <v>A</v>
+        <v>64</v>
       </c>
       <c r="C3" s="5" t="str">
         <f>DEC2BIN(A3)</f>
-        <v>1010</v>
+        <v>1100100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5">
         <f>HEX2DEC(A5)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5" t="str">
         <f>HEX2BIN(A5)</f>
-        <v>1011</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="str">
         <f>DEC2HEX(D10)</f>
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="E9" s="5">
         <f>HEX2DEC(D9)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F9" s="5" t="str">
         <f>HEX2BIN(D9)</f>
-        <v>1010</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <f>HEX2DEC(B9)</f>
-        <v>9</v>
+        <v>2074</v>
       </c>
       <c r="C10">
         <f>HEX2DEC(C9)</f>
-        <v>1</v>
+        <v>2061</v>
       </c>
       <c r="D10">
         <f>IF(A9="+",B10+C10,IF(A9="-",B10-C10,IF(A9="*",B10*C10,IF(A9="/",B10/C10,0))))</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -625,26 +632,26 @@
     <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9" xr:uid="{4A2A55A2-1A60-460E-831D-7FA79752C144}">
       <formula1>$A$14:$A$17</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
C64 VICII Improvement when reading raster position. Real read moment happens at the very end of the any LD? instruction which takes a couple of cycles. At the same time the raster is moving and could jump to another line. If that jump happened before the max cycles of the instruction the value read should be the new raster position actually. It didn't happen with the current implementation. Now it has been addressed, but in a generical way. CPU is now a Notifier too and notifies an event about the instruction that is about to execute, That notification can be capture (in the case of the C64 implementation) from the Computer class to inform the VICII to (Chip) to consider this cycles difference. Additionally minor errors in the way the debug info is generated have been sorted out as well.
</commit_message>
<xml_diff>
--- a/docs/HexaDec.xlsx
+++ b/docs/HexaDec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326A4F39-2EEE-4977-9B7B-7A2B123A2E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EA7097-99BE-4BF8-ABB8-18202CF80491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{C70C2E63-9336-4B10-BFD2-FFF09962B0E6}"/>
   </bookViews>
@@ -77,13 +77,13 @@
     <t>Binary</t>
   </si>
   <si>
-    <t>080d</t>
-  </si>
-  <si>
-    <t>081a</t>
-  </si>
-  <si>
     <t>0d</t>
+  </si>
+  <si>
+    <t>d000</t>
+  </si>
+  <si>
+    <t>d800</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5">
         <f>HEX2DEC(A5)</f>
@@ -595,57 +595,54 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D9" s="5" t="str">
         <f>DEC2HEX(D10)</f>
-        <v>D</v>
+        <v>800</v>
       </c>
       <c r="E9" s="5">
         <f>HEX2DEC(D9)</f>
-        <v>13</v>
-      </c>
-      <c r="F9" s="5" t="str">
+        <v>2048</v>
+      </c>
+      <c r="F9" s="5" t="e">
         <f>HEX2BIN(D9)</f>
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <f>HEX2DEC(B9)</f>
-        <v>2074</v>
+        <v>55296</v>
       </c>
       <c r="C10">
         <f>HEX2DEC(C9)</f>
-        <v>2061</v>
+        <v>53248</v>
       </c>
       <c r="D10">
         <f>IF(A9="+",B10+C10,IF(A9="-",B10-C10,IF(A9="*",B10*C10,IF(A9="/",B10/C10,0))))</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
C64 VICII. Error in all drawing routines (chars and sprites). Specially in the ones multicolor. Because this error the chars and sprites multicolor were drawn in blocks of 2 pixels. When srolling the effect was not fully smooth. F6500. The Flag not used is set to 1 as is usually defined in all documentation. Now is possible to draw a cyan square around the sprites when GRIDON COLOR ON command is used.
</commit_message>
<xml_diff>
--- a/docs/HexaDec.xlsx
+++ b/docs/HexaDec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\EMULATORS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EA7097-99BE-4BF8-ABB8-18202CF80491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7966123-0ED0-40E8-BBF9-5F7880BBF028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{C70C2E63-9336-4B10-BFD2-FFF09962B0E6}"/>
   </bookViews>
@@ -80,10 +80,10 @@
     <t>0d</t>
   </si>
   <si>
-    <t>d000</t>
-  </si>
-  <si>
-    <t>d800</t>
+    <t>fc</t>
+  </si>
+  <si>
+    <t>fd</t>
   </si>
 </sst>
 </file>
@@ -530,15 +530,15 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5" t="str">
         <f>DEC2HEX(A3)</f>
-        <v>64</v>
+        <v>A</v>
       </c>
       <c r="C3" s="5" t="str">
         <f>DEC2BIN(A3)</f>
-        <v>1100100</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -592,7 +592,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
@@ -602,29 +602,29 @@
       </c>
       <c r="D9" s="5" t="str">
         <f>DEC2HEX(D10)</f>
-        <v>800</v>
+        <v>1F9</v>
       </c>
       <c r="E9" s="5">
         <f>HEX2DEC(D9)</f>
-        <v>2048</v>
-      </c>
-      <c r="F9" s="5" t="e">
+        <v>505</v>
+      </c>
+      <c r="F9" s="5" t="str">
         <f>HEX2BIN(D9)</f>
-        <v>#NUM!</v>
+        <v>111111001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <f>HEX2DEC(B9)</f>
-        <v>55296</v>
+        <v>253</v>
       </c>
       <c r="C10">
         <f>HEX2DEC(C9)</f>
-        <v>53248</v>
+        <v>252</v>
       </c>
       <c r="D10">
         <f>IF(A9="+",B10+C10,IF(A9="-",B10-C10,IF(A9="*",B10*C10,IF(A9="/",B10/C10,0))))</f>
-        <v>2048</v>
+        <v>505</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">

</xml_diff>